<commit_message>
Pengerjaan import data excel stok tabung, pemakaian oksigen, sample, pendataan, dan kasus
</commit_message>
<xml_diff>
--- a/repository/template/import_data_kasus.xlsx
+++ b/repository/template/import_data_kasus.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Kab/Kota</t>
   </si>
@@ -110,6 +110,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -140,14 +143,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,45 +435,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pengerjaan import data excel pada control kamar, dan vaksinasi, dan perbaikan coding pada control dan module kamar
</commit_message>
<xml_diff>
--- a/repository/template/import_data_kasus.xlsx
+++ b/repository/template/import_data_kasus.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="KabKota" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Pengerjaan control dan module capaian vaksinasi
</commit_message>
<xml_diff>
--- a/repository/template/import_data_kasus.xlsx
+++ b/repository/template/import_data_kasus.xlsx
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,97 +478,97 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>